<commit_message>
Adicionei arquivos no gitignore
</commit_message>
<xml_diff>
--- a/dadosNACA.xlsx
+++ b/dadosNACA.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
   </bookViews>
   <sheets>
     <sheet name="DadosNACA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="6">
   <si>
     <t>NACA</t>
   </si>
@@ -99,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -219,13 +219,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -271,10 +306,43 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -604,18 +672,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="10.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:11">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -631,8 +700,26 @@
       <c r="E1" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
@@ -642,14 +729,32 @@
       <c r="C2" s="11">
         <v>10000</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="17">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="11">
+        <v>20000</v>
+      </c>
+      <c r="F2" s="17">
+        <v>40000</v>
+      </c>
+      <c r="G2" s="11">
+        <v>40000</v>
+      </c>
+      <c r="H2" s="17">
+        <v>80000</v>
+      </c>
+      <c r="I2" s="11">
+        <v>80000</v>
+      </c>
+      <c r="J2" s="17">
         <v>160000</v>
       </c>
-      <c r="E2" s="11">
+      <c r="K2" s="11">
         <v>160000</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:11">
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
@@ -665,8 +770,26 @@
       <c r="E3" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -676,14 +799,32 @@
       <c r="C4" s="3">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="18">
         <v>0</v>
       </c>
       <c r="E4" s="3">
+        <v>2.4500000000000001E-2</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:11">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -693,14 +834,32 @@
       <c r="C5" s="3">
         <v>3.3799999999999997E-2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="18">
+        <v>0.1057</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2.47E-2</v>
+      </c>
+      <c r="F5" s="18">
         <v>0.11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="G5" s="3">
+        <v>1.77E-2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.34E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="K5" s="3">
         <v>1.04E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:11">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -710,14 +869,32 @@
       <c r="C6" s="3">
         <v>3.4299999999999997E-2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="18">
+        <v>0.2072</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="F6" s="18">
         <v>0.22</v>
       </c>
-      <c r="E6" s="3">
+      <c r="G6" s="3">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="K6" s="3">
         <v>1.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:11">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -727,14 +904,32 @@
       <c r="C7" s="3">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="18">
+        <v>0.30320000000000003</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="F7" s="18">
+        <v>0.33760000000000001</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H7" s="18">
         <v>0.33</v>
       </c>
-      <c r="E7" s="3">
+      <c r="I7" s="3">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="K7" s="3">
         <v>1.14E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:11">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -744,14 +939,32 @@
       <c r="C8" s="3">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="18">
+        <v>0.39290000000000003</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0.44640000000000002</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="H8" s="18">
         <v>0.44</v>
       </c>
-      <c r="E8" s="3">
+      <c r="I8" s="3">
+        <v>1.55E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="K8" s="3">
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:11">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -761,14 +974,32 @@
       <c r="C9" s="3">
         <v>3.5099999999999999E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="18">
+        <v>0.47810000000000002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0.52759999999999996</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.18E-2</v>
+      </c>
+      <c r="H9" s="18">
         <v>0.55000000000000004</v>
       </c>
-      <c r="E9" s="3">
+      <c r="I9" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K9" s="3">
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:11">
       <c r="A10" s="6">
         <v>6</v>
       </c>
@@ -778,14 +1009,32 @@
       <c r="C10" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="18">
+        <v>-2.98E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.61160000000000003</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.62839999999999996</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.89E-2</v>
+      </c>
+      <c r="J10" s="2">
         <v>0.66</v>
       </c>
-      <c r="E10" s="3">
+      <c r="K10" s="3">
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:11">
       <c r="A11" s="6">
         <v>7</v>
       </c>
@@ -795,14 +1044,32 @@
       <c r="C11" s="3">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="18">
+        <v>-0.1089</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="F11" s="18">
+        <v>-2.12E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.72270000000000001</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="J11" s="2">
         <v>0.746</v>
       </c>
-      <c r="E11" s="3">
+      <c r="K11" s="3">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:11">
       <c r="A12" s="6">
         <v>8</v>
       </c>
@@ -812,14 +1079,32 @@
       <c r="C12" s="3">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="18">
+        <v>-6.9900000000000004E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F12" s="18">
+        <v>-6.1499999999999999E-2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="J12" s="2">
         <v>0.82740000000000002</v>
       </c>
-      <c r="E12" s="3">
+      <c r="K12" s="3">
         <v>1.8499999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:11">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -829,14 +1114,32 @@
       <c r="C13" s="3">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="18">
+        <v>-1.9800000000000002E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F13" s="18">
+        <v>-1.6E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="H13" s="18">
+        <v>-1E-3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="J13" s="2">
         <v>0.85270000000000001</v>
       </c>
-      <c r="E13" s="3">
+      <c r="K13" s="3">
         <v>2.0299999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:11">
       <c r="A14" s="6">
         <v>10</v>
       </c>
@@ -846,14 +1149,32 @@
       <c r="C14" s="3">
         <v>0.10100000000000001</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="18">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="F14" s="18">
+        <v>3.44E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H14" s="18">
+        <v>4.1300000000000003E-2</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="J14" s="2">
         <v>0.13250000000000001</v>
       </c>
-      <c r="E14" s="3">
+      <c r="K14" s="3">
         <v>1.8800000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:11">
       <c r="A15" s="6">
         <v>11</v>
       </c>
@@ -863,14 +1184,32 @@
       <c r="C15" s="3">
         <v>0.11700000000000001</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="18">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="F15" s="18">
+        <v>8.6900000000000005E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="H15" s="18">
+        <v>9.11E-2</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J15" s="2">
         <v>0.1095</v>
       </c>
-      <c r="E15" s="3">
+      <c r="K15" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:11">
       <c r="A16" s="6">
         <v>12</v>
       </c>
@@ -880,14 +1219,32 @@
       <c r="C16" s="3">
         <v>0.13400000000000001</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.15329999999999999</v>
+      <c r="D16" s="18">
+        <v>0.18940000000000001</v>
       </c>
       <c r="E16" s="3">
         <v>0.13400000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="18">
+        <v>0.1406</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="H16" s="18">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="6">
         <v>13</v>
       </c>
@@ -897,14 +1254,32 @@
       <c r="C17" s="3">
         <v>0.152</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.20300000000000001</v>
+      <c r="D17" s="18">
+        <v>0.19339999999999999</v>
       </c>
       <c r="E17" s="3">
         <v>0.152</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="18">
+        <v>0.19450000000000001</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.152</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.1966</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.152</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="6">
         <v>14</v>
       </c>
@@ -914,14 +1289,32 @@
       <c r="C18" s="3">
         <v>0.17100000000000001</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.25459999999999999</v>
+      <c r="D18" s="18">
+        <v>0.24740000000000001</v>
       </c>
       <c r="E18" s="3">
         <v>0.17100000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="18">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.25040000000000001</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.25459999999999999</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.17100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="6">
         <v>15</v>
       </c>
@@ -931,14 +1324,32 @@
       <c r="C19" s="3">
         <v>0.19</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="18">
+        <v>0.3014</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.191</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0.3024</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0.30430000000000001</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="J19" s="2">
         <v>0.30819999999999997</v>
       </c>
-      <c r="E19" s="3">
+      <c r="K19" s="3">
         <v>0.19</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:11">
       <c r="A20" s="6">
         <v>16</v>
       </c>
@@ -948,14 +1359,32 @@
       <c r="C20" s="3">
         <v>0.21</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.36199999999999999</v>
+      <c r="D20" s="18">
+        <v>0.35539999999999999</v>
       </c>
       <c r="E20" s="3">
         <v>0.21</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="18">
+        <v>0.35630000000000001</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="H20" s="18">
+        <v>0.35820000000000002</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="6">
         <v>17</v>
       </c>
@@ -965,14 +1394,32 @@
       <c r="C21" s="3">
         <v>0.23100000000000001</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="18">
+        <v>0.40889999999999999</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="F21" s="18">
+        <v>0.41070000000000001</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="J21" s="2">
         <v>0.42</v>
       </c>
-      <c r="E21" s="3">
+      <c r="K21" s="3">
         <v>0.23100000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:11">
       <c r="A22" s="6">
         <v>18</v>
       </c>
@@ -982,14 +1429,32 @@
       <c r="C22" s="3">
         <v>0.252</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.4768</v>
+      <c r="D22" s="18">
+        <v>0.46200000000000002</v>
       </c>
       <c r="E22" s="3">
         <v>0.252</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="18">
+        <v>0.46439999999999998</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.252</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0.46889999999999998</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.252</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.4768</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" s="6">
         <v>19</v>
       </c>
@@ -999,14 +1464,32 @@
       <c r="C23" s="3">
         <v>0.27400000000000002</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.53220000000000001</v>
+      <c r="D23" s="18">
+        <v>0.51470000000000005</v>
       </c>
       <c r="E23" s="3">
         <v>0.27400000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="18">
+        <v>0.51780000000000004</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="H23" s="18">
+        <v>0.5232</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.53220000000000001</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.27400000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="6">
         <v>20</v>
       </c>
@@ -1016,14 +1499,32 @@
       <c r="C24" s="3">
         <v>0.29699999999999999</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.58699999999999997</v>
+      <c r="D24" s="18">
+        <v>0.56630000000000003</v>
       </c>
       <c r="E24" s="3">
         <v>0.29699999999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="18">
+        <v>0.57079999999999997</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="H24" s="18">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="6">
         <v>21</v>
       </c>
@@ -1033,14 +1534,32 @@
       <c r="C25" s="3">
         <v>0.32</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.64139999999999997</v>
+      <c r="D25" s="18">
+        <v>0.61839999999999995</v>
       </c>
       <c r="E25" s="3">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="18">
+        <v>0.62319999999999998</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0.63049999999999995</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.64139999999999997</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" s="6">
         <v>22</v>
       </c>
@@ -1050,14 +1569,32 @@
       <c r="C26" s="3">
         <v>0.34399999999999997</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.6956</v>
+      <c r="D26" s="18">
+        <v>0.67090000000000005</v>
       </c>
       <c r="E26" s="3">
         <v>0.34399999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="18">
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0.68389999999999995</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0.6956</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" s="6">
         <v>23</v>
       </c>
@@ -1067,14 +1604,32 @@
       <c r="C27" s="3">
         <v>0.36899999999999999</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.74970000000000003</v>
+      <c r="D27" s="18">
+        <v>0.7238</v>
       </c>
       <c r="E27" s="3">
         <v>0.36899999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="18">
+        <v>0.72829999999999995</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0.73729999999999996</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" s="6">
         <v>24</v>
       </c>
@@ -1084,14 +1639,32 @@
       <c r="C28" s="3">
         <v>0.39400000000000002</v>
       </c>
-      <c r="D28" s="2">
-        <v>0.8034</v>
+      <c r="D28" s="18">
+        <v>0.77649999999999997</v>
       </c>
       <c r="E28" s="3">
         <v>0.39400000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="18">
+        <v>0.78090000000000004</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0.79020000000000001</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.8034</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.39400000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" s="6">
         <v>25</v>
       </c>
@@ -1101,14 +1674,32 @@
       <c r="C29" s="3">
         <v>0.42</v>
       </c>
-      <c r="D29" s="2">
-        <v>0.85719999999999996</v>
+      <c r="D29" s="18">
+        <v>0.82969999999999999</v>
       </c>
       <c r="E29" s="3">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="18">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="H29" s="18">
+        <v>0.84319999999999995</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.85719999999999996</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" s="6">
         <v>26</v>
       </c>
@@ -1118,14 +1709,32 @@
       <c r="C30" s="3">
         <v>0.44600000000000001</v>
       </c>
-      <c r="D30" s="2">
-        <v>0.91090000000000004</v>
+      <c r="D30" s="18">
+        <v>0.8831</v>
       </c>
       <c r="E30" s="3">
         <v>0.44600000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="18">
+        <v>0.88729999999999998</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="H30" s="18">
+        <v>0.89629999999999999</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.91090000000000004</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="6">
         <v>27</v>
       </c>
@@ -1135,14 +1744,32 @@
       <c r="C31" s="3">
         <v>0.47299999999999998</v>
       </c>
-      <c r="D31" s="2">
-        <v>0.96460000000000001</v>
+      <c r="D31" s="18">
+        <v>0.9365</v>
       </c>
       <c r="E31" s="3">
         <v>0.47299999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="18">
+        <v>0.94069999999999998</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="H31" s="18">
+        <v>0.9496</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.96460000000000001</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" s="6">
         <v>30</v>
       </c>
@@ -1152,14 +1779,32 @@
       <c r="C32" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="18">
         <v>0.91500000000000004</v>
       </c>
       <c r="E32" s="3">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="18">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H32" s="18">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="6">
         <v>35</v>
       </c>
@@ -1169,14 +1814,32 @@
       <c r="C33" s="3">
         <v>0.745</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="18">
         <v>1.02</v>
       </c>
       <c r="E33" s="3">
         <v>0.745</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="18">
+        <v>1.02</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0.745</v>
+      </c>
+      <c r="H33" s="18">
+        <v>1.02</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.745</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="6">
         <v>40</v>
       </c>
@@ -1186,14 +1849,32 @@
       <c r="C34" s="3">
         <v>0.92</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="18">
         <v>1.075</v>
       </c>
       <c r="E34" s="3">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="18">
+        <v>1.075</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="H34" s="18">
+        <v>1.075</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1.075</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="6">
         <v>45</v>
       </c>
@@ -1203,14 +1884,32 @@
       <c r="C35" s="3">
         <v>1.075</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="18">
         <v>1.085</v>
       </c>
       <c r="E35" s="3">
         <v>1.075</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="18">
+        <v>1.085</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.075</v>
+      </c>
+      <c r="H35" s="18">
+        <v>1.085</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.075</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.085</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1.075</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="6">
         <v>50</v>
       </c>
@@ -1220,14 +1919,32 @@
       <c r="C36" s="3">
         <v>1.2150000000000001</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="18">
         <v>1.04</v>
       </c>
       <c r="E36" s="3">
         <v>1.2150000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="18">
+        <v>1.04</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="H36" s="18">
+        <v>1.04</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1.2150000000000001</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1.04</v>
+      </c>
+      <c r="K36" s="3">
+        <v>1.2150000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
       <c r="A37" s="6">
         <v>55</v>
       </c>
@@ -1237,14 +1954,32 @@
       <c r="C37" s="3">
         <v>1.345</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="18">
         <v>0.96499999999999997</v>
       </c>
       <c r="E37" s="3">
         <v>1.345</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="18">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1.345</v>
+      </c>
+      <c r="H37" s="18">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.345</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="K37" s="3">
+        <v>1.345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
       <c r="A38" s="6">
         <v>60</v>
       </c>
@@ -1254,14 +1989,32 @@
       <c r="C38" s="3">
         <v>1.47</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="18">
         <v>0.875</v>
       </c>
       <c r="E38" s="3">
         <v>1.47</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="18">
+        <v>0.875</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1.47</v>
+      </c>
+      <c r="H38" s="18">
+        <v>0.875</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.47</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.875</v>
+      </c>
+      <c r="K38" s="3">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="6">
         <v>65</v>
       </c>
@@ -1271,14 +2024,32 @@
       <c r="C39" s="3">
         <v>1.575</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="18">
         <v>0.76500000000000001</v>
       </c>
       <c r="E39" s="3">
         <v>1.575</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="18">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1.575</v>
+      </c>
+      <c r="H39" s="18">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1.575</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="K39" s="3">
+        <v>1.575</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
       <c r="A40" s="6">
         <v>70</v>
       </c>
@@ -1288,14 +2059,32 @@
       <c r="C40" s="3">
         <v>1.665</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="18">
         <v>0.65</v>
       </c>
       <c r="E40" s="3">
         <v>1.665</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="18">
+        <v>0.65</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1.665</v>
+      </c>
+      <c r="H40" s="18">
+        <v>0.65</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.665</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1.665</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
       <c r="A41" s="6">
         <v>75</v>
       </c>
@@ -1305,14 +2094,32 @@
       <c r="C41" s="3">
         <v>1.7350000000000001</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="18">
         <v>0.51500000000000001</v>
       </c>
       <c r="E41" s="3">
+        <v>1.734</v>
+      </c>
+      <c r="F41" s="18">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="G41" s="3">
         <v>1.7350000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="H41" s="18">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1.7350000000000001</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="K41" s="3">
+        <v>1.7350000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
       <c r="A42" s="6">
         <v>80</v>
       </c>
@@ -1322,14 +2129,32 @@
       <c r="C42" s="3">
         <v>1.78</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="18">
         <v>0.37</v>
       </c>
       <c r="E42" s="3">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1.78</v>
+      </c>
+      <c r="H42" s="18">
+        <v>0.37</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1.78</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="K42" s="3">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
       <c r="A43" s="6">
         <v>85</v>
       </c>
@@ -1339,14 +2164,32 @@
       <c r="C43" s="3">
         <v>1.8</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="18">
         <v>0.22</v>
       </c>
       <c r="E43" s="3">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="H43" s="18">
+        <v>0.22</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
       <c r="A44" s="6">
         <v>90</v>
       </c>
@@ -1356,14 +2199,32 @@
       <c r="C44" s="3">
         <v>1.8</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E44" s="3">
         <v>1.8</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="H44" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="J44" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K44" s="3">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
       <c r="A45" s="6">
         <v>95</v>
       </c>
@@ -1373,14 +2234,32 @@
       <c r="C45" s="3">
         <v>1.78</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="18">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="E45" s="3">
         <v>1.78</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="18">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1.78</v>
+      </c>
+      <c r="H45" s="18">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.78</v>
+      </c>
+      <c r="J45" s="2">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="K45" s="3">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
       <c r="A46" s="6">
         <v>100</v>
       </c>
@@ -1390,14 +2269,32 @@
       <c r="C46" s="3">
         <v>1.75</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="18">
         <v>-0.22</v>
       </c>
       <c r="E46" s="3">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="18">
+        <v>-0.22</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="H46" s="18">
+        <v>-0.22</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="J46" s="2">
+        <v>-0.22</v>
+      </c>
+      <c r="K46" s="3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
       <c r="A47" s="6">
         <v>105</v>
       </c>
@@ -1407,14 +2304,32 @@
       <c r="C47" s="3">
         <v>1.7</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="18">
         <v>-0.37</v>
       </c>
       <c r="E47" s="3">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="18">
+        <v>-0.37</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="H47" s="18">
+        <v>-0.37</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="J47" s="2">
+        <v>-0.37</v>
+      </c>
+      <c r="K47" s="3">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
       <c r="A48" s="6">
         <v>110</v>
       </c>
@@ -1424,14 +2339,32 @@
       <c r="C48" s="3">
         <v>1.635</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="18">
         <v>-0.51</v>
       </c>
       <c r="E48" s="3">
         <v>1.635</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="18">
+        <v>-0.51</v>
+      </c>
+      <c r="G48" s="3">
+        <v>1.635</v>
+      </c>
+      <c r="H48" s="18">
+        <v>-0.51</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1.635</v>
+      </c>
+      <c r="J48" s="2">
+        <v>-0.51</v>
+      </c>
+      <c r="K48" s="3">
+        <v>1.635</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
       <c r="A49" s="6">
         <v>115</v>
       </c>
@@ -1441,14 +2374,32 @@
       <c r="C49" s="3">
         <v>1.5549999999999999</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="18">
         <v>-0.625</v>
       </c>
       <c r="E49" s="3">
         <v>1.5549999999999999</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="18">
+        <v>-0.625</v>
+      </c>
+      <c r="G49" s="3">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="H49" s="18">
+        <v>-0.625</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="J49" s="2">
+        <v>-0.625</v>
+      </c>
+      <c r="K49" s="3">
+        <v>1.5549999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
       <c r="A50" s="6">
         <v>120</v>
       </c>
@@ -1458,14 +2409,32 @@
       <c r="C50" s="3">
         <v>1.4650000000000001</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="18">
         <v>-0.73499999999999999</v>
       </c>
       <c r="E50" s="3">
+        <v>1.464</v>
+      </c>
+      <c r="F50" s="18">
+        <v>-0.73499999999999999</v>
+      </c>
+      <c r="G50" s="3">
         <v>1.4650000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="H50" s="18">
+        <v>-0.73499999999999999</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.4650000000000001</v>
+      </c>
+      <c r="J50" s="2">
+        <v>-0.73499999999999999</v>
+      </c>
+      <c r="K50" s="3">
+        <v>1.4650000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
       <c r="A51" s="6">
         <v>125</v>
       </c>
@@ -1475,14 +2444,32 @@
       <c r="C51" s="3">
         <v>1.35</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="18">
         <v>-0.84</v>
       </c>
       <c r="E51" s="3">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="18">
+        <v>-0.84</v>
+      </c>
+      <c r="G51" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="H51" s="18">
+        <v>-0.84</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="J51" s="2">
+        <v>-0.84</v>
+      </c>
+      <c r="K51" s="3">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="6">
         <v>130</v>
       </c>
@@ -1492,14 +2479,32 @@
       <c r="C52" s="3">
         <v>1.2250000000000001</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="18">
         <v>-0.91</v>
       </c>
       <c r="E52" s="3">
         <v>1.2250000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="18">
+        <v>-0.91</v>
+      </c>
+      <c r="G52" s="3">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="H52" s="18">
+        <v>-0.91</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="J52" s="2">
+        <v>-0.91</v>
+      </c>
+      <c r="K52" s="3">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="A53" s="6">
         <v>135</v>
       </c>
@@ -1509,14 +2514,32 @@
       <c r="C53" s="3">
         <v>1.085</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="18">
         <v>-0.94499999999999995</v>
       </c>
       <c r="E53" s="3">
         <v>1.085</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="18">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="G53" s="3">
+        <v>1.085</v>
+      </c>
+      <c r="H53" s="18">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1.085</v>
+      </c>
+      <c r="J53" s="2">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="K53" s="3">
+        <v>1.085</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54" s="6">
         <v>140</v>
       </c>
@@ -1526,14 +2549,32 @@
       <c r="C54" s="3">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="18">
         <v>-0.94499999999999995</v>
       </c>
       <c r="E54" s="3">
         <v>0.92500000000000004</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="18">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="H54" s="18">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="J54" s="2">
+        <v>-0.94499999999999995</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.92500000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
       <c r="A55" s="6">
         <v>145</v>
       </c>
@@ -1543,14 +2584,32 @@
       <c r="C55" s="3">
         <v>0.755</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="18">
         <v>-0.91</v>
       </c>
       <c r="E55" s="3">
         <v>0.755</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="18">
+        <v>-0.91</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.755</v>
+      </c>
+      <c r="H55" s="18">
+        <v>-0.91</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0.755</v>
+      </c>
+      <c r="J55" s="2">
+        <v>-0.91</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" s="6">
         <v>150</v>
       </c>
@@ -1560,14 +2619,32 @@
       <c r="C56" s="3">
         <v>0.57499999999999996</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="18">
         <v>-0.85</v>
       </c>
       <c r="E56" s="3">
         <v>0.57499999999999996</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="18">
+        <v>-0.85</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H56" s="18">
+        <v>-0.85</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="J56" s="2">
+        <v>-0.85</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0.57499999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" s="6">
         <v>155</v>
       </c>
@@ -1577,14 +2654,32 @@
       <c r="C57" s="3">
         <v>0.42</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="18">
         <v>-0.74</v>
       </c>
       <c r="E57" s="3">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="18">
+        <v>-0.74</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="H57" s="18">
+        <v>-0.74</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0.42</v>
+      </c>
+      <c r="J57" s="2">
+        <v>-0.74</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="A58" s="6">
         <v>160</v>
       </c>
@@ -1594,14 +2689,32 @@
       <c r="C58" s="3">
         <v>0.32</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="18">
         <v>-0.66</v>
       </c>
       <c r="E58" s="3">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="18">
+        <v>-0.66</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="H58" s="18">
+        <v>-0.66</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="J58" s="2">
+        <v>-0.66</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="A59" s="6">
         <v>165</v>
       </c>
@@ -1611,14 +2724,32 @@
       <c r="C59" s="3">
         <v>0.23</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="18">
         <v>-0.67500000000000004</v>
       </c>
       <c r="E59" s="3">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="18">
+        <v>-0.67500000000000004</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="H59" s="18">
+        <v>-0.67500000000000004</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="J59" s="2">
+        <v>-0.67500000000000004</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
       <c r="A60" s="6">
         <v>170</v>
       </c>
@@ -1628,14 +2759,32 @@
       <c r="C60" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="18">
         <v>-0.85</v>
       </c>
       <c r="E60" s="3">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="18">
+        <v>-0.85</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H60" s="18">
+        <v>-0.85</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J60" s="2">
+        <v>-0.85</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" s="6">
         <v>175</v>
       </c>
@@ -1645,14 +2794,32 @@
       <c r="C61" s="3">
         <v>5.5E-2</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="18">
         <v>-0.69</v>
       </c>
       <c r="E61" s="3">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="18">
+        <v>-0.69</v>
+      </c>
+      <c r="G61" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H61" s="18">
+        <v>-0.69</v>
+      </c>
+      <c r="I61" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="J61" s="2">
+        <v>-0.69</v>
+      </c>
+      <c r="K61" s="3">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="A62" s="7">
         <v>180</v>
       </c>
@@ -1666,6 +2833,24 @@
         <v>0</v>
       </c>
       <c r="E62" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H62" s="4">
+        <v>0</v>
+      </c>
+      <c r="I62" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0</v>
+      </c>
+      <c r="K62" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcao da interpolacao por alfa e Re; calculo de 0 a 360
</commit_message>
<xml_diff>
--- a/dadosNACA.xlsx
+++ b/dadosNACA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="DadosNACA" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -885,7 +885,7 @@
         <v>0.22</v>
       </c>
       <c r="I6" s="3">
-        <v>0.13800000000000001</v>
+        <v>1.38E-2</v>
       </c>
       <c r="J6" s="2">
         <v>0.22</v>

</xml_diff>